<commit_message>
Added module 0622 dispenser
</commit_message>
<xml_diff>
--- a/LAB_20200622_0_Dispenser/LAB_20200622_0_Dispenser.xlsx
+++ b/LAB_20200622_0_Dispenser/LAB_20200622_0_Dispenser.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a59c1bdb761853cd/NAER/EELAB/EELAB/LAB_20200622_0_Dispenser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="237" documentId="11_F25DC773A252ABDACC1048E0995B61245BDE58ED" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9650B604-6184-45AF-8040-C9F81EE41EED}"/>
+  <xr:revisionPtr revIDLastSave="281" documentId="11_F25DC773A252ABDACC1048E0995B61245BDE58ED" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{748D823E-D4F0-4D7E-9908-FE9918E8E270}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1296" yWindow="276" windowWidth="15408" windowHeight="12084" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SystemDiagram" sheetId="1" r:id="rId1"/>
@@ -2144,16 +2144,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2168,7 +2168,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4495800" y="3101340"/>
+          <a:off x="9608820" y="3124200"/>
           <a:ext cx="533400" cy="487680"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2204,16 +2204,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2228,7 +2228,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6560820" y="3124200"/>
+          <a:off x="11673840" y="3147060"/>
           <a:ext cx="533400" cy="487680"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2264,16 +2264,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2288,7 +2288,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5074920" y="3337560"/>
+          <a:off x="10187940" y="3360420"/>
           <a:ext cx="1424940" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2317,16 +2317,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>487680</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2341,7 +2341,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="5074920" y="3520440"/>
+          <a:off x="10187940" y="3543300"/>
           <a:ext cx="1447800" cy="7620"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2370,10 +2370,10 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1144159" cy="275909"/>
     <xdr:sp macro="" textlink="">
@@ -2389,7 +2389,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5219700" y="3070860"/>
+          <a:off x="10332720" y="3093720"/>
           <a:ext cx="1144159" cy="275909"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2441,10 +2441,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1144159" cy="275909"/>
     <xdr:sp macro="" textlink="">
@@ -2460,7 +2460,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5219700" y="3543300"/>
+          <a:off x="10332720" y="3566160"/>
           <a:ext cx="1144159" cy="275909"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2512,9 +2512,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1708416" cy="275909"/>
@@ -2531,7 +2531,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="876300" y="952500"/>
+          <a:off x="1691640" y="1714500"/>
           <a:ext cx="1708416" cy="275909"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2569,7 +2569,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
-            <a:t>連續出水</a:t>
+            <a:t>連續供水</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
@@ -2583,10 +2583,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1313180" cy="275909"/>
     <xdr:sp macro="" textlink="">
@@ -2602,7 +2602,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1645920" y="1905000"/>
+          <a:off x="6156960" y="2354580"/>
           <a:ext cx="1313180" cy="275909"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2633,6 +2633,472 @@
           <a:r>
             <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
             <a:t>設定出水時間長度</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2217145" cy="275909"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="文字方塊 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF53424C-5232-46EA-AE42-D428150C9A7C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1546860" y="2590800"/>
+          <a:ext cx="2217145" cy="275909"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
+            <a:t>檢查</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>"</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
+            <a:t>連續</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>"</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
+            <a:t>鍵是否按下</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
+            <a:t>上緣觸發</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="748923" cy="275909"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="文字方塊 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41D76582-0C90-447F-B093-0B836E31C9E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1043940" y="4160520"/>
+          <a:ext cx="748923" cy="275909"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US"/>
+            <a:t>一般供水</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="748923" cy="275909"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="文字方塊 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B066D04-F3BD-4B99-93B6-0955508AA5D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3291840" y="4191000"/>
+          <a:ext cx="748923" cy="275909"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US"/>
+            <a:t>連續供水</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2217145" cy="275909"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="文字方塊 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE02921C-BC8F-4EB7-9EDF-47D49BE65409}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1546860" y="2887980"/>
+          <a:ext cx="2217145" cy="275909"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
+            <a:t>檢查</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>"</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
+            <a:t>出水</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>"</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
+            <a:t>鍵是否按下</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
+            <a:t>上緣觸發</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="466794" cy="275909"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="文字方塊 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B596779-128E-4DF9-9BFE-C6AA557FBF33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3810000" y="4739640"/>
+          <a:ext cx="466794" cy="275909"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
+            <a:t>供水</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="748923" cy="275909"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="文字方塊 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3739494F-BD0E-40CE-A088-849EA57172C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2819400" y="4709160"/>
+          <a:ext cx="748923" cy="275909"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US" sz="1100"/>
+            <a:t>停止供水</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1031051" cy="275909"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="文字方塊 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3A43AC9-4378-4346-8CFB-1D186CC596F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1882140" y="5814060"/>
+          <a:ext cx="1031051" cy="275909"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-TW" altLang="en-US"/>
+            <a:t>紀錄按鍵狀態</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2989,8 +3455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAAB7E6-D1C5-4163-8B6E-601D8518EFE8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -3005,8 +3471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F73A6051-291B-495D-A6CC-4CC1DF5BC627}">
   <dimension ref="A5:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -3411,6 +3877,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>